<commit_message>
add obTIME and obTIMEend to the template
add obTIME and obTIMEend to the template
</commit_message>
<xml_diff>
--- a/accdcTemplateOutsideSubmission.xlsx
+++ b/accdcTemplateOutsideSubmission.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\03 - RESOURCES\AC CDC Data Load\outsideSubmissionTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53042441-90AA-4AF7-AA73-F302DB6EDFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A69B265-7F75-4316-B789-E3481B6EB9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14505" yWindow="240" windowWidth="14055" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9105" yWindow="5025" windowWidth="19860" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,9 @@
     <sheet name="PROTOCOL" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AV$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AX$2</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>REFNUM</t>
   </si>
@@ -256,14 +256,21 @@
   </si>
   <si>
     <t>eBird - Incidental</t>
+  </si>
+  <si>
+    <t>OBTIME</t>
+  </si>
+  <si>
+    <t>OBTIMEend</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="hh:mm"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -318,6 +325,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -347,7 +355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -374,6 +382,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -691,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AV2"/>
+  <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AR9" sqref="AR9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -704,49 +724,50 @@
     <col min="3" max="3" width="6.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="9.42578125" style="9" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11" style="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.42578125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11" style="9" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17" style="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9" style="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11" style="9" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17" style="9" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="9" style="9" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="8.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9" style="9" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="5.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="8.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="10" style="9" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="49" max="16384" width="8.85546875" style="9"/>
+    <col min="34" max="34" width="8.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9" style="9" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="8.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="7.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9" style="9" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="5.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10" style="9" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="51" max="16384" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="2" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:50" s="2" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -771,128 +792,134 @@
       <c r="H1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AL1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AN1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AO1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AP1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AR1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AT1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AV1" s="5" t="s">
+      <c r="AX1" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:48" s="8" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:50" s="8" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -901,20 +928,20 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
@@ -941,10 +968,12 @@
       <c r="AT2" s="1"/>
       <c r="AU2" s="1"/>
       <c r="AV2" s="1"/>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AV2" xr:uid="{8EF81207-EAEC-4F51-84D0-DB07B3DAFBD3}"/>
-  <dataValidations count="16">
+  <autoFilter ref="A1:AX2" xr:uid="{8EF81207-EAEC-4F51-84D0-DB07B3DAFBD3}"/>
+  <dataValidations count="15">
     <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="yyyy2 must have text length = 4._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="E1:E1048576" xr:uid="{8759099F-EA84-471E-810A-FFCB466A1148}">
       <formula1>4</formula1>
     </dataValidation>
@@ -955,31 +984,31 @@
       <formula1>1</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" error="LATDEC must have a minimum value of -90 and a maximum value of 90._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="O1:O1048576" xr:uid="{3E3B9040-D53D-4EE4-9942-FD2F4C08E301}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" error="LATDEC must have a minimum value of -90 and a maximum value of 90._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="Q1:Q1048576" xr:uid="{3E3B9040-D53D-4EE4-9942-FD2F4C08E301}">
       <formula1>-90</formula1>
       <formula2>90</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LONDEC2 must have a minimum value of -180 and a maximum value of 180._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="R1:R1048576" xr:uid="{E0963D9F-8EB3-4CAE-9972-F3B4443DD9B2}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LONDEC2 must have a minimum value of -180 and a maximum value of 180._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="T1:T1048576" xr:uid="{E0963D9F-8EB3-4CAE-9972-F3B4443DD9B2}">
       <formula1>-180</formula1>
       <formula2>180</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LATDEC2 must have a minimum value of -90 and a maximum value of 90._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="Q1:Q1048576" xr:uid="{8EC441BF-CE69-46B2-B117-8DB4DFCF4E67}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LATDEC2 must have a minimum value of -90 and a maximum value of 90._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="S1:S1048576" xr:uid="{8EC441BF-CE69-46B2-B117-8DB4DFCF4E67}">
       <formula1>-90</formula1>
       <formula2>90</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LOCUNCM must be a whole number greater than or equal to 10._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="T1:T1048576" xr:uid="{76877D72-6D7B-4053-9D8A-EF5817DEA169}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LOCUNCM must be a whole number greater than or equal to 10._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="V1:V1048576" xr:uid="{76877D72-6D7B-4053-9D8A-EF5817DEA169}">
       <formula1>10</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="YYYY must have text length = 4._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="B1:B1048576" xr:uid="{2B2538EA-15F5-4C6F-9BD7-FFFB59409F9B}">
       <formula1>4</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="ELEVmin must be a whole number greater than or equal to 0._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="AA1:AA1048576" xr:uid="{9DF3AC12-B532-4B95-9071-2B1B0EC4A8B0}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="ELEVmin must be a whole number greater than or equal to 0._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="AC1:AC1048576" xr:uid="{9DF3AC12-B532-4B95-9071-2B1B0EC4A8B0}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Lowercase text only._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="AJ1:AJ1048576" xr:uid="{A03A87E5-1A90-4590-9340-BE069CE30FCB}">
-      <formula1>EXACT(LOWER(AJ1),AJ1)</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="COLLDUP must be a whole number greater than 0._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="AS1:AS1048576" xr:uid="{C625A903-796B-43AF-B42E-C1CBF9B064D4}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Lowercase text only._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="AK1:AL1048576" xr:uid="{A03A87E5-1A90-4590-9340-BE069CE30FCB}">
+      <formula1>EXACT(LOWER(AK1),AK1)</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="COLLDUP must be a whole number greater than 0._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="AU1:AU1048576" xr:uid="{C625A903-796B-43AF-B42E-C1CBF9B064D4}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="MM must have a minimum text length of 1 and a maximum text length of 2._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="C1:C1048576" xr:uid="{63AA1352-24B0-40CA-9C2F-ED3E31036D5C}">
@@ -994,12 +1023,9 @@
       <formula1>1</formula1>
       <formula2>2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LONDEC must have a minimum value of -180 and a maximum value of 180._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="P1:P1048576" xr:uid="{FBE1E6CF-FE6A-454F-8063-F9B3175370DC}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="LONDEC must have a minimum value of -180 and a maximum value of 180._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="R1:R1048576" xr:uid="{FBE1E6CF-FE6A-454F-8063-F9B3175370DC}">
       <formula1>-180</formula1>
       <formula2>180</formula2>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Lowercase text only._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" sqref="AI1:AI1048576" xr:uid="{44753312-9CC3-4B87-AD48-40F3BCBEBFCA}">
-      <formula1>EXACT(LOWER(AI1),AI1)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1011,25 +1037,25 @@
           <x14:formula1>
             <xm:f>OBEVID!$A$1:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>AB1:AB1048576</xm:sqref>
+          <xm:sqref>AD1:AD1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="This value is not allowed in the OBABUN field. See the OBABUN tab for allowable values._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" xr:uid="{535D8599-9410-414A-8279-5DBB317BAB6C}">
           <x14:formula1>
             <xm:f>OBABUN!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>AC1:AC1048576</xm:sqref>
+          <xm:sqref>AE1:AE1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="This value is not allowed in the OBABUNSITE field. See the OBABUNSITE tab for allowable values._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" xr:uid="{281AA0A5-0C44-4F74-9371-6C6F2D49754A}">
           <x14:formula1>
             <xm:f>OBABUNSITE!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>AD1:AD1048576</xm:sqref>
+          <xm:sqref>AF1:AF1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="This value is not allowed in the PROTOCOL field. See the PROTOCOL tab for allowable values._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" xr:uid="{2DBE70EF-0781-49B6-9F67-E70BF08A9C65}">
           <x14:formula1>
             <xm:f>PROTOCOL!$A$1:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>AP1:AP1048576</xm:sqref>
+          <xm:sqref>AR1:AR1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
update template file with README sheet and version number on template sheet
</commit_message>
<xml_diff>
--- a/accdcTemplateOutsideSubmission.xlsx
+++ b/accdcTemplateOutsideSubmission.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\03 - RESOURCES\AC CDC Data Load\outsideSubmissionTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\01 - PROJECTS\537_observationTemplate\outsideSubmissionTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A69B265-7F75-4316-B789-E3481B6EB9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE00C4D-9D98-4828-B723-4CC6E638F494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9105" yWindow="5025" windowWidth="19860" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13005" yWindow="1080" windowWidth="15795" windowHeight="15120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="OBEVID" sheetId="2" r:id="rId2"/>
-    <sheet name="OBABUN" sheetId="3" r:id="rId3"/>
-    <sheet name="OBABUNSITE" sheetId="4" r:id="rId4"/>
-    <sheet name="PROTOCOL" sheetId="5" r:id="rId5"/>
+    <sheet name="template_v0-00" sheetId="1" r:id="rId1"/>
+    <sheet name="README" sheetId="6" r:id="rId2"/>
+    <sheet name="OBEVID" sheetId="2" r:id="rId3"/>
+    <sheet name="OBABUN" sheetId="3" r:id="rId4"/>
+    <sheet name="OBABUNSITE" sheetId="4" r:id="rId5"/>
+    <sheet name="PROTOCOL" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AX$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'template_v0-00'!$A$1:$AX$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>REFNUM</t>
   </si>
@@ -262,6 +263,18 @@
   </si>
   <si>
     <t>OBTIMEend</t>
+  </si>
+  <si>
+    <t>to find metadata associated with this template ("data dictionary"), go to our repo: https://github.com/atlanticcanadacdc/outsideSubmissionTemplate</t>
+  </si>
+  <si>
+    <t>to make sure you have to most up-to-date version, download this file directly from our repo: https://github.com/atlanticcanadacdc/outsideSubmissionTemplate</t>
+  </si>
+  <si>
+    <t>to provide feedback on this template, please submit this Google form</t>
+  </si>
+  <si>
+    <t>or create an issue on the issue tracker</t>
   </si>
 </sst>
 </file>
@@ -272,7 +285,7 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="hh:mm"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,6 +340,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -351,11 +372,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -396,8 +418,10 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{4397B092-219E-4F51-867E-8E15B030440A}"/>
   </cellStyles>
@@ -713,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1064,6 +1088,48 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B0B503C-45C2-4682-A279-7D9876A20A9B}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="to make sure you have to most up to date version, download this file from our repo: https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" xr:uid="{6915430C-55DD-436F-A74B-E2345D056ECD}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{68273A7E-5932-4AB3-916D-F05551D05E2C}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{FA7FC906-4AAA-411C-83EE-13BA40AD1AF7}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{4045D2E4-E1DA-4C81-BF39-5ED34065FEC4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB774BC8-9194-4144-975B-CFE4E7E3F552}">
   <dimension ref="A1:A10"/>
   <sheetViews>
@@ -1129,7 +1195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3900AA5-948C-4FE1-9D24-5854C30EABD8}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -1164,7 +1230,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED745171-8CAD-48CA-A70F-98F1CC85585B}">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -1194,7 +1260,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7DD475-3512-455B-8B60-40854C146542}">
   <dimension ref="A1:A7"/>
   <sheetViews>

</xml_diff>